<commit_message>
Fix Protocol Liquidation Fee calculation (#185)
Fix Protocol Liquidation Fee calculation.
</commit_message>
<xml_diff>
--- a/contracts/credit-manager/tests/files/Rover - Dynamic LB & CF test cases v1.1.xlsx
+++ b/contracts/credit-manager/tests/files/Rover - Dynamic LB & CF test cases v1.1.xlsx
@@ -1047,12 +1047,12 @@
         <v>38</v>
       </c>
       <c r="C41" s="11">
-        <f>CEILING(FLOOR(C40*C27,1)*C5,1)</f>
-        <v>1</v>
+        <f>FLOOR(CEILING(FLOOR(D38*C27,1)*C5,1)/D13,1)</f>
+        <v>4</v>
       </c>
       <c r="D41" s="11">
         <f>FLOOR(C41*D13,1)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="42">
@@ -1061,7 +1061,7 @@
       </c>
       <c r="C42" s="11">
         <f>C40-C41</f>
-        <v>2631</v>
+        <v>2628</v>
       </c>
       <c r="D42" s="11">
         <f>FLOOR(C42*D13,1)</f>
@@ -1158,7 +1158,7 @@
       </c>
       <c r="C55" s="11">
         <f>C42</f>
-        <v>2631</v>
+        <v>2628</v>
       </c>
     </row>
   </sheetData>
@@ -1209,7 +1209,7 @@
         <v>2</v>
       </c>
       <c r="C5" s="3">
-        <v>0.02</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="6">
@@ -1579,7 +1579,7 @@
       </c>
       <c r="F26" s="15">
         <f>D26+C47</f>
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="G26" s="18"/>
     </row>
@@ -1753,12 +1753,12 @@
         <v>38</v>
       </c>
       <c r="C46" s="11">
-        <f>CEILING(FLOOR(C45*C32,1)*C5,1)</f>
-        <v>1</v>
+        <f>FLOOR(CEILING(FLOOR(D43*C32,1)*C5,1)/F13,1)</f>
+        <v>7</v>
       </c>
       <c r="D46" s="11">
         <f>FLOOR(C46*F13,1)</f>
-        <v>9</v>
+        <v>69</v>
       </c>
     </row>
     <row r="47">
@@ -1767,11 +1767,11 @@
       </c>
       <c r="C47" s="11">
         <f>C45-C46</f>
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="D47" s="11">
         <f>FLOOR(C47*F13,1)</f>
-        <v>1945</v>
+        <v>1885</v>
       </c>
     </row>
     <row r="48">
@@ -1838,7 +1838,7 @@
         <v>2</v>
       </c>
       <c r="C5" s="3">
-        <v>0.02</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="6">
@@ -2233,7 +2233,7 @@
       </c>
       <c r="F26" s="15">
         <f>D26+C47</f>
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="G26" s="18"/>
     </row>
@@ -2407,12 +2407,12 @@
         <v>38</v>
       </c>
       <c r="C46" s="11">
-        <f>CEILING(FLOOR(C40*C32,1)*C5,1)</f>
-        <v>1</v>
+        <f>FLOOR(CEILING(FLOOR(D43*C32,1)*C5,1)/H13,1)</f>
+        <v>3</v>
       </c>
       <c r="D46" s="11">
         <f>FLOOR(C46*H13,1)</f>
-        <v>9</v>
+        <v>29</v>
       </c>
     </row>
     <row r="47">
@@ -2421,11 +2421,11 @@
       </c>
       <c r="C47" s="11">
         <f>C45-C46</f>
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D47" s="11">
         <f>FLOOR(C47*H13,1)</f>
-        <v>868</v>
+        <v>849</v>
       </c>
     </row>
     <row r="48">
@@ -2886,12 +2886,12 @@
         <v>38</v>
       </c>
       <c r="C41" s="11">
-        <f>CEILING(FLOOR(C40*C27,1)*C5,1)</f>
-        <v>1</v>
+        <f>FLOOR(CEILING(FLOOR(D38*C27,1)*C5,1)/D13,1)</f>
+        <v>4</v>
       </c>
       <c r="D41" s="11">
         <f>FLOOR(C41*D13,1)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="42">
@@ -2900,7 +2900,7 @@
       </c>
       <c r="C42" s="11">
         <f>C40-C41</f>
-        <v>971</v>
+        <v>968</v>
       </c>
       <c r="D42" s="11">
         <f>FLOOR(C42*D13,1)</f>
@@ -3016,7 +3016,7 @@
       </c>
       <c r="C57" s="11">
         <f>C42</f>
-        <v>971</v>
+        <v>968</v>
       </c>
     </row>
   </sheetData>
@@ -3459,12 +3459,12 @@
         <v>38</v>
       </c>
       <c r="C41" s="11">
-        <f>CEILING(FLOOR(C40*C27,1)*C5,1)</f>
-        <v>1</v>
+        <f>FLOOR(CEILING(FLOOR(D38*C27,1)*C5,1)/D13,1)</f>
+        <v>4</v>
       </c>
       <c r="D41" s="11">
         <f>FLOOR(C41*D13,1)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="42">
@@ -3473,7 +3473,7 @@
       </c>
       <c r="C42" s="11">
         <f>C40-C41</f>
-        <v>2975</v>
+        <v>2972</v>
       </c>
       <c r="D42" s="11">
         <f>FLOOR(C42*D13,1)</f>
@@ -3570,7 +3570,7 @@
       </c>
       <c r="C55" s="11">
         <f>C42</f>
-        <v>2975</v>
+        <v>2972</v>
       </c>
     </row>
   </sheetData>
@@ -4014,12 +4014,12 @@
         <v>38</v>
       </c>
       <c r="C41" s="11">
-        <f>CEILING(FLOOR(C40*C27,1)*C5,1)</f>
-        <v>1</v>
+        <f>FLOOR(CEILING(FLOOR(D38*C27,1)*C5,1)/D13,1)</f>
+        <v>4</v>
       </c>
       <c r="D41" s="11">
         <f>FLOOR(C41*D13,1)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="42">
@@ -4028,7 +4028,7 @@
       </c>
       <c r="C42" s="11">
         <f>C40-C41</f>
-        <v>2391</v>
+        <v>2388</v>
       </c>
       <c r="D42" s="11">
         <f>FLOOR(C42*D13,1)</f>
@@ -4125,7 +4125,7 @@
       </c>
       <c r="C55" s="11">
         <f>C42</f>
-        <v>2391</v>
+        <v>2388</v>
       </c>
     </row>
   </sheetData>
@@ -4570,12 +4570,12 @@
         <v>38</v>
       </c>
       <c r="C41" s="11">
-        <f>CEILING(FLOOR(C40*C27,1)*C5,1)</f>
-        <v>3</v>
+        <f>FLOOR(CEILING(FLOOR(D38*C27,1)*C5,1)/D13,1)</f>
+        <v>4</v>
       </c>
       <c r="D41" s="11">
         <f>FLOOR(C41*D13,1)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="42">
@@ -4584,7 +4584,7 @@
       </c>
       <c r="C42" s="11">
         <f>C40-C41</f>
-        <v>1229</v>
+        <v>1228</v>
       </c>
       <c r="D42" s="11">
         <f>FLOOR(C42*D13,1)</f>
@@ -4700,7 +4700,7 @@
       </c>
       <c r="C57" s="11">
         <f>C42</f>
-        <v>1229</v>
+        <v>1228</v>
       </c>
     </row>
   </sheetData>
@@ -5186,11 +5186,11 @@
       </c>
       <c r="F28" s="15">
         <f>D28+C49</f>
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="G28" s="17">
         <f>F28-1</f>
-        <v>402</v>
+        <v>399</v>
       </c>
       <c r="H28" s="8" t="s">
         <v>54</v>
@@ -5358,12 +5358,12 @@
         <v>38</v>
       </c>
       <c r="C48" s="11">
-        <f>CEILING(FLOOR(C47*C34,1)*C5,1)</f>
-        <v>1</v>
+        <f>FLOOR(CEILING(FLOOR(D45*C34,1)*C5,1)/F13,1)</f>
+        <v>4</v>
       </c>
       <c r="D48" s="11">
         <f>FLOOR(C48*F13,1)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="49">
@@ -5372,7 +5372,7 @@
       </c>
       <c r="C49" s="11">
         <f>C47-C48</f>
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="D49" s="11">
         <f>FLOOR(C49*F13,1)</f>
@@ -6049,7 +6049,7 @@
         <v>38</v>
       </c>
       <c r="C48" s="11">
-        <f>CEILING(FLOOR(C47*C34,1)*C5,1)</f>
+        <f>FLOOR(CEILING(FLOOR(D45*C34,1)*C5,1)/F13,1)</f>
         <v>1</v>
       </c>
       <c r="D48" s="11">
@@ -6134,7 +6134,7 @@
         <v>2</v>
       </c>
       <c r="C5" s="3">
-        <v>0.02</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="6">
@@ -6677,7 +6677,7 @@
         <v>38</v>
       </c>
       <c r="C46" s="11">
-        <f>CEILING(FLOOR(C45*C32,1)*C5,1)</f>
+        <f>FLOOR(CEILING(FLOOR(D43*C32,1)*C5,1)/F13,1)</f>
         <v>1</v>
       </c>
       <c r="D46" s="11">
@@ -6762,7 +6762,7 @@
         <v>2</v>
       </c>
       <c r="C5" s="3">
-        <v>0.02</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="6">
@@ -7305,7 +7305,7 @@
         <v>38</v>
       </c>
       <c r="C46" s="11">
-        <f>CEILING(FLOOR(C45*C32,1)*C5,1)</f>
+        <f>FLOOR(CEILING(FLOOR(D43*C32,1)*C5,1)/F13,1)</f>
         <v>1</v>
       </c>
       <c r="D46" s="11">

</xml_diff>